<commit_message>
separando responsabilidades de control del nodo de las gramaticas para que sea mas facil extender
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -443,7 +443,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>2.6</v>
+        <v>6.95</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2.6</v>
+        <v>6.95</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2.6</v>
+        <v>6.95</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
reemplazando libreria js-pattern porque no resulto muy potente
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Hoja1" state="show" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>tag</t>
   </si>
@@ -52,14 +52,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,7 +82,9 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -402,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="1" customWidth="1"/>
@@ -443,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>3.65</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -464,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>3.65</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -485,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3.65</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
@@ -522,8 +524,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(AND(B6&gt;3,B6&lt;7),"presion no estable","presion estable")</f>
+        <v>presion no estable</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agragando analizador sintactico antlr. intepreta la gramatica, pero no opera
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>

</xml_diff>

<commit_message>
tratando de resolver gramatica usando 'grammar comprises production code'
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>tag</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -573,6 +573,27 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(5=6,"presion no estable","presion estable")</f>
+        <v>presion estable</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>

</xml_diff>

<commit_message>
agregando parser implementado con antlr y soporte de una pila externa para controlar las operaciones en los distintos niveles donde unificaba. debe existir solucion nativa en antlr para ello, pero no se pudo hacer funcionar (posiblementes usar visitors)
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>1.8</v>
+        <v>7.45</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>1.8</v>
+        <v>7.45</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>1.8</v>
+        <v>7.45</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>

</xml_diff>

<commit_message>
las planillas con extension xls no funcionan con la libreria utilizada, tiene que ser xlsx
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -515,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
se agregan detalles de implementacion al readme, y se deja terminada la presentacion de datos desde planilla en el editor de nodos de node-red, aunque no fue posible completar las filas con datos verdaderos, falta experiencia o un caso de ejemplo sobre como hacer push desde el server hacia el front en un nodo node-red
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -414,7 +414,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>7.45</v>
+        <v>3.95</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>7.45</v>
+        <v>3.95</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>7.45</v>
+        <v>3.95</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
@@ -515,7 +515,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>7.45</v>
+        <v>3.95</v>
       </c>
       <c r="C5" s="1">
         <v>6.8</v>
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
agregando comentarios de uso en readme
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas.xlsx
+++ b/Final/dominio/formulas.xlsx
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>6.85</v>
+        <v>5.15</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>6.85</v>
+        <v>5.15</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>6.85</v>
+        <v>5.15</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
@@ -515,7 +515,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>6.85</v>
+        <v>5.15</v>
       </c>
       <c r="C5" s="1">
         <v>6.8</v>

</xml_diff>